<commit_message>
Updated README to include information on MMRP
</commit_message>
<xml_diff>
--- a/code/NSS75 Variable List.xlsx
+++ b/code/NSS75 Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF5B35B-43A4-475E-B768-5A7B068D560A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B9F8CF-E186-495C-993B-0FD9E919E792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{AAF0233B-02C2-403C-A73B-396F7A361711}"/>
   </bookViews>
@@ -771,7 +771,7 @@
   <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3421,7 +3421,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>